<commit_message>
XLS macros extended, documented implemented error handling if some module has linkage error
</commit_message>
<xml_diff>
--- a/jamal-xls/src/test/resources/test.xlsx
+++ b/jamal-xls/src/test/resources/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/verhasp/github/jamal/jamal-xls/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514FBA5B-A136-5645-98B1-9209F59CADED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FBA03A-C10E-0242-99B9-767B4DF1045D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2640" windowWidth="28040" windowHeight="17440" xr2:uid="{5FA2AFD4-335A-3246-B938-841A5EE25EAD}"/>
   </bookViews>
@@ -501,20 +501,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4AEB8E2-D051-7446-9F43-E52F39AB36A8}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -522,7 +522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <f>A1+A2</f>
         <v>3</v>
@@ -530,8 +530,11 @@
       <c r="C3">
         <v>53.2</v>
       </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>_xlfn.CONCAT(A1,A2,A3)</f>
         <v>123</v>
@@ -540,7 +543,7 @@
         <v>45441</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>7</v>
       </c>

</xml_diff>